<commit_message>
GUI app update. gen weights and fill grups added
</commit_message>
<xml_diff>
--- a/Filled_Groups.xlsx
+++ b/Filled_Groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="101">
   <si>
     <t>Prezime</t>
   </si>
@@ -34,298 +34,289 @@
     <t>Grupa</t>
   </si>
   <si>
-    <t>Bošnjak</t>
-  </si>
-  <si>
-    <t>Katarina</t>
-  </si>
-  <si>
-    <t>kbosnj00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23130115</t>
-  </si>
-  <si>
-    <t>kbosnj00</t>
-  </si>
-  <si>
-    <t>G1 - UTO 14:15 - 17:00 (A326)</t>
-  </si>
-  <si>
-    <t>Burić</t>
-  </si>
-  <si>
-    <t>Ilija</t>
-  </si>
-  <si>
-    <t>iburic01@fesb.hr</t>
-  </si>
-  <si>
-    <t>23137894</t>
-  </si>
-  <si>
-    <t>iburic01</t>
-  </si>
-  <si>
-    <t>Duždević</t>
-  </si>
-  <si>
-    <t>Domagoj</t>
-  </si>
-  <si>
-    <t>dduzde00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23146869</t>
-  </si>
-  <si>
-    <t>dduzde00</t>
-  </si>
-  <si>
-    <t>Erceg</t>
-  </si>
-  <si>
-    <t>Boris</t>
-  </si>
-  <si>
-    <t>berceg01@fesb.hr</t>
-  </si>
-  <si>
-    <t>23137709</t>
-  </si>
-  <si>
-    <t>berceg01</t>
-  </si>
-  <si>
-    <t>Falak</t>
-  </si>
-  <si>
-    <t>Monika</t>
-  </si>
-  <si>
-    <t>mfalak00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23141152</t>
-  </si>
-  <si>
-    <t>mfalak00</t>
-  </si>
-  <si>
-    <t>Gardijan</t>
+    <t>Barbača</t>
+  </si>
+  <si>
+    <t>Tomislav</t>
+  </si>
+  <si>
+    <t>tbarba00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23162754</t>
+  </si>
+  <si>
+    <t>tbarba00</t>
+  </si>
+  <si>
+    <t>G1 - PON 09:30 - 11:00 (B419)</t>
+  </si>
+  <si>
+    <t>Barbir</t>
+  </si>
+  <si>
+    <t>Dalmatino</t>
+  </si>
+  <si>
+    <t>dbarbi00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23151631</t>
+  </si>
+  <si>
+    <t>dbarbi00</t>
+  </si>
+  <si>
+    <t>Barić</t>
+  </si>
+  <si>
+    <t>Damjana</t>
+  </si>
+  <si>
+    <t>dbaric01@fesb.hr</t>
+  </si>
+  <si>
+    <t>177054411</t>
+  </si>
+  <si>
+    <t>dbaric01</t>
+  </si>
+  <si>
+    <t>Bebić</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>ibebic00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23160055</t>
+  </si>
+  <si>
+    <t>ibebic00</t>
+  </si>
+  <si>
+    <t>Biloš</t>
+  </si>
+  <si>
+    <t>Mateo</t>
+  </si>
+  <si>
+    <t>mbilos02@fesb.hr</t>
+  </si>
+  <si>
+    <t>23144021</t>
+  </si>
+  <si>
+    <t>mbilos02</t>
+  </si>
+  <si>
+    <t>Bitunjac</t>
+  </si>
+  <si>
+    <t>Luka</t>
+  </si>
+  <si>
+    <t>lbitun00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23146853</t>
+  </si>
+  <si>
+    <t>lbitun00</t>
+  </si>
+  <si>
+    <t>Brčić</t>
+  </si>
+  <si>
+    <t>Mijo</t>
+  </si>
+  <si>
+    <t>mbrcic00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23128183</t>
+  </si>
+  <si>
+    <t>mbrcic00</t>
+  </si>
+  <si>
+    <t>Brkić</t>
   </si>
   <si>
     <t>Marko</t>
   </si>
   <si>
-    <t>mgardi00@fesb.hr</t>
-  </si>
-  <si>
-    <t>66310423</t>
-  </si>
-  <si>
-    <t>mgardi00</t>
-  </si>
-  <si>
-    <t>Hegedić</t>
-  </si>
-  <si>
-    <t>Josip</t>
-  </si>
-  <si>
-    <t>jheged00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23143211</t>
-  </si>
-  <si>
-    <t>jheged00</t>
-  </si>
-  <si>
-    <t>Ivanković</t>
-  </si>
-  <si>
-    <t>mivank00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23135431</t>
-  </si>
-  <si>
-    <t>mivank00</t>
-  </si>
-  <si>
-    <t>Juranović</t>
-  </si>
-  <si>
-    <t>Nina</t>
-  </si>
-  <si>
-    <t>njuran00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23137714</t>
-  </si>
-  <si>
-    <t>njuran00</t>
-  </si>
-  <si>
-    <t>Kotromanović</t>
-  </si>
-  <si>
-    <t>jkotro00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23143477</t>
-  </si>
-  <si>
-    <t>jkotro00</t>
-  </si>
-  <si>
-    <t>Martinović</t>
-  </si>
-  <si>
-    <t>Martina</t>
-  </si>
-  <si>
-    <t>mmarti01@fesb.hr</t>
-  </si>
-  <si>
-    <t>23149626</t>
-  </si>
-  <si>
-    <t>mmarti01</t>
-  </si>
-  <si>
-    <t>Matić</t>
-  </si>
-  <si>
-    <t>Magdalena</t>
-  </si>
-  <si>
-    <t>mmatic04@fesb.hr</t>
-  </si>
-  <si>
-    <t>23149673</t>
-  </si>
-  <si>
-    <t>mmatic04</t>
-  </si>
-  <si>
-    <t>Roko</t>
-  </si>
-  <si>
-    <t>rmatic00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23149717</t>
-  </si>
-  <si>
-    <t>rmatic00</t>
-  </si>
-  <si>
-    <t>Mihalj</t>
-  </si>
-  <si>
-    <t>Kristijan</t>
-  </si>
-  <si>
-    <t>kmihal01@fesb.hr</t>
-  </si>
-  <si>
-    <t>23138160</t>
-  </si>
-  <si>
-    <t>kmihal01</t>
-  </si>
-  <si>
-    <t>Ozretić</t>
-  </si>
-  <si>
-    <t>Marin</t>
-  </si>
-  <si>
-    <t>mozret00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23143050</t>
-  </si>
-  <si>
-    <t>mozret00</t>
-  </si>
-  <si>
-    <t>Sabljić</t>
-  </si>
-  <si>
-    <t>Vatroslav</t>
-  </si>
-  <si>
-    <t>vsablj00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23153662</t>
-  </si>
-  <si>
-    <t>vsablj00</t>
-  </si>
-  <si>
-    <t>Sesar</t>
-  </si>
-  <si>
-    <t>Ronaldo</t>
-  </si>
-  <si>
-    <t>rsesar00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23147567</t>
-  </si>
-  <si>
-    <t>rsesar00</t>
-  </si>
-  <si>
-    <t>Tolić</t>
-  </si>
-  <si>
-    <t>Bože</t>
-  </si>
-  <si>
-    <t>btolic00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23150426</t>
-  </si>
-  <si>
-    <t>btolic00</t>
-  </si>
-  <si>
-    <t>Vidić</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>ividic00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23150356</t>
-  </si>
-  <si>
-    <t>ividic00</t>
-  </si>
-  <si>
-    <t>Vuković</t>
-  </si>
-  <si>
-    <t>Geni</t>
-  </si>
-  <si>
-    <t>gvukov00@fesb.hr</t>
-  </si>
-  <si>
-    <t>23150629</t>
-  </si>
-  <si>
-    <t>gvukov00</t>
+    <t>mbrkic01@fesb.hr</t>
+  </si>
+  <si>
+    <t>23144180</t>
+  </si>
+  <si>
+    <t>mbrkic01</t>
+  </si>
+  <si>
+    <t>Budimir</t>
+  </si>
+  <si>
+    <t>Ante</t>
+  </si>
+  <si>
+    <t>abudim02@fesb.hr</t>
+  </si>
+  <si>
+    <t>23160013</t>
+  </si>
+  <si>
+    <t>abudim02</t>
+  </si>
+  <si>
+    <t>Bulat</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>dbulat01@fesb.hr</t>
+  </si>
+  <si>
+    <t>23159089</t>
+  </si>
+  <si>
+    <t>dbulat01</t>
+  </si>
+  <si>
+    <t>Bušić</t>
+  </si>
+  <si>
+    <t>Marino</t>
+  </si>
+  <si>
+    <t>mbusic00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23158718</t>
+  </si>
+  <si>
+    <t>mbusic00</t>
+  </si>
+  <si>
+    <t>Cikojević</t>
+  </si>
+  <si>
+    <t>Matej</t>
+  </si>
+  <si>
+    <t>mcikoj00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23162567</t>
+  </si>
+  <si>
+    <t>mcikoj00</t>
+  </si>
+  <si>
+    <t>Češljar</t>
+  </si>
+  <si>
+    <t>iceslj00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23162268</t>
+  </si>
+  <si>
+    <t>iceslj00</t>
+  </si>
+  <si>
+    <t>G2 - PON 11:00 - 12:30 (B419)</t>
+  </si>
+  <si>
+    <t>Čondić</t>
+  </si>
+  <si>
+    <t>Mihael</t>
+  </si>
+  <si>
+    <t>mcondi02@fesb.hr</t>
+  </si>
+  <si>
+    <t>23162476</t>
+  </si>
+  <si>
+    <t>mcondi02</t>
+  </si>
+  <si>
+    <t>Čović</t>
+  </si>
+  <si>
+    <t>Borna</t>
+  </si>
+  <si>
+    <t>bcovic00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23160188</t>
+  </si>
+  <si>
+    <t>bcovic00</t>
+  </si>
+  <si>
+    <t>Čuljak</t>
+  </si>
+  <si>
+    <t>lculja00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23133806</t>
+  </si>
+  <si>
+    <t>lculja00</t>
+  </si>
+  <si>
+    <t>Ćurković</t>
+  </si>
+  <si>
+    <t>Lorena</t>
+  </si>
+  <si>
+    <t>lcurko01@fesb.hr</t>
+  </si>
+  <si>
+    <t>23152030</t>
+  </si>
+  <si>
+    <t>lcurko01</t>
+  </si>
+  <si>
+    <t>Domazet</t>
+  </si>
+  <si>
+    <t>Dario</t>
+  </si>
+  <si>
+    <t>ddomaz01@fesb.hr</t>
+  </si>
+  <si>
+    <t>23159101</t>
+  </si>
+  <si>
+    <t>ddomaz01</t>
+  </si>
+  <si>
+    <t>Dubravčić Radolović</t>
+  </si>
+  <si>
+    <t>Korina</t>
+  </si>
+  <si>
+    <t>kdubra00@fesb.hr</t>
+  </si>
+  <si>
+    <t>23153017</t>
+  </si>
+  <si>
+    <t>kdubra00</t>
   </si>
 </sst>
 </file>
@@ -657,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -828,16 +819,16 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>
@@ -845,19 +836,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -865,19 +856,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -885,19 +876,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -905,19 +896,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -925,162 +916,142 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
         <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>